<commit_message>
Rettet abstract og kapitel 1
</commit_message>
<xml_diff>
--- a/Exceltalmums.xlsx
+++ b/Exceltalmums.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="21">
   <si>
     <t>a_1</t>
   </si>
@@ -75,6 +75,18 @@
   </si>
   <si>
     <t>2.4</t>
+  </si>
+  <si>
+    <t>1,83M</t>
+  </si>
+  <si>
+    <t>3.68</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>2,24M</t>
   </si>
 </sst>
 </file>
@@ -400,11 +412,12 @@
   <dimension ref="B2:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="20" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -912,6 +925,30 @@
       </c>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>5.5</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1E-4</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>2</v>
+      </c>
+      <c r="J15">
+        <v>0.01</v>
+      </c>
+      <c r="K15">
+        <v>1E-4</v>
+      </c>
+      <c r="L15">
+        <v>-4.9999999999999998E-7</v>
+      </c>
       <c r="O15">
         <v>3</v>
       </c>
@@ -921,8 +958,41 @@
       <c r="Q15">
         <v>1</v>
       </c>
+      <c r="S15" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <v>0.01</v>
+      </c>
+      <c r="K16">
+        <v>1E-4</v>
+      </c>
+      <c r="L16">
+        <v>-4.9999999999999998E-7</v>
+      </c>
       <c r="O16">
         <v>3</v>
       </c>
@@ -932,8 +1002,38 @@
       <c r="Q16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="S16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="T16" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J17">
+        <v>3.0000000000000001E-6</v>
+      </c>
+      <c r="K17">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="L17">
+        <v>4.9999999999999998E-7</v>
+      </c>
       <c r="O17" s="1">
         <v>3.3096291507664799</v>
       </c>
@@ -943,8 +1043,41 @@
       <c r="Q17" s="1">
         <v>1.15373917406258</v>
       </c>
-    </row>
-    <row r="18" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="S17" s="2">
+        <v>3.84</v>
+      </c>
+      <c r="T17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18">
+        <v>5.5</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>1E-4</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>0.01</v>
+      </c>
+      <c r="K18">
+        <v>1E-4</v>
+      </c>
+      <c r="L18">
+        <v>-4.9999999999999998E-7</v>
+      </c>
       <c r="O18">
         <v>3</v>
       </c>
@@ -954,8 +1087,14 @@
       <c r="Q18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="S18" s="2">
+        <v>3.68</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="O19">
         <v>3</v>
       </c>

</xml_diff>